<commit_message>
fixed protocols 30 mex delay period
</commit_message>
<xml_diff>
--- a/protocol_andy_sensory_20150814.xlsx
+++ b/protocol_andy_sensory_20150814.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200"/>
+    <workbookView xWindow="20880" yWindow="3140" windowWidth="16380" windowHeight="8200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -96,17 +96,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="A1:I3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -490,47 +498,317 @@
         <v>25</v>
       </c>
       <c r="F2">
-        <v>60000</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>30</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <f>(D2*E2+F2)*H2+G2*1000</f>
-        <v>290000</v>
+        <f t="shared" ref="I2:I12" si="0">(D2*E2+F2)*H2+G2*1000</f>
+        <v>35000</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="F3">
-        <v>60000</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-      <c r="H3">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <f>(D3*E3+F3)*H3+G3*1000</f>
-        <v>290000</v>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>25</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>200</v>
+      </c>
+      <c r="E11">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>200</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>60</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>65000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>